<commit_message>
I Have no idea what am i doing...
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tk-hdd-backup\Data\@KMUTNB WORKs\Year 1\040613201 Computer Programming 1\ComPro1Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582EFB52-CCF7-44E7-BE45-D5BB45B10FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E20F48-9D4B-4FE4-832D-3CBB444A2E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{17119E70-600C-4351-8F05-AAB983F732AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Q</t>
   </si>
@@ -126,13 +126,16 @@
   </si>
   <si>
     <t>Answer:</t>
+  </si>
+  <si>
+    <t>Stats</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,13 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -303,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,25 +345,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -670,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC46F51D-D48B-4786-B218-0052D0D1623D}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,54 +718,55 @@
       <c r="U1" s="4"/>
       <c r="V1" s="5"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
       <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
       <c r="V3" s="7"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -933,33 +947,29 @@
       <c r="P16" s="10"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="V17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="14" t="s">
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="12"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="14"/>
       <c r="V18" s="7"/>
-      <c r="Z18" s="17"/>
-      <c r="AA18" s="17"/>
-    </row>
-    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V19" s="7"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="17"/>
-    </row>
-    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
         <v>0</v>
       </c>
@@ -1001,10 +1011,8 @@
       </c>
       <c r="U20" s="10"/>
       <c r="V20" s="7"/>
-      <c r="Z20" s="17"/>
-      <c r="AA20" s="17"/>
-    </row>
-    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1026,11 +1034,8 @@
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="7"/>
-      <c r="Z21" s="17"/>
-      <c r="AA21" s="17"/>
-      <c r="AB21" s="17"/>
-    </row>
-    <row r="22" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="10" t="s">
         <v>10</v>
       </c>
@@ -1068,34 +1073,29 @@
       </c>
       <c r="T22" s="10"/>
       <c r="V22" s="7"/>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="17"/>
-    </row>
-    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
       <c r="V23" s="7"/>
-      <c r="AA23" s="17"/>
-      <c r="AB23" s="17"/>
-    </row>
-    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
         <v>26</v>
       </c>
@@ -1136,8 +1136,7 @@
       <c r="U24" s="10"/>
       <c r="V24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1160,7 +1159,7 @@
       <c r="U25" s="10"/>
       <c r="V25" s="7"/>
     </row>
-    <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1185,27 +1184,35 @@
       <c r="V26" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:P18"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="H20:I21"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="Q22:R23"/>
-    <mergeCell ref="S22:T23"/>
-    <mergeCell ref="N20:O21"/>
-    <mergeCell ref="P20:Q21"/>
-    <mergeCell ref="R20:S21"/>
-    <mergeCell ref="T20:U21"/>
-    <mergeCell ref="G22:H23"/>
-    <mergeCell ref="I22:J23"/>
-    <mergeCell ref="K22:L23"/>
-    <mergeCell ref="M22:N23"/>
-    <mergeCell ref="O22:P23"/>
-    <mergeCell ref="B2:U3"/>
+  <mergeCells count="62">
+    <mergeCell ref="I2:N3"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="O7:P8"/>
     <mergeCell ref="O24:P25"/>
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="B24:D25"/>
@@ -1221,32 +1228,25 @@
     <mergeCell ref="M15:N16"/>
     <mergeCell ref="C22:D23"/>
     <mergeCell ref="E22:F23"/>
-    <mergeCell ref="O5:P6"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="K22:L23"/>
+    <mergeCell ref="M22:N23"/>
+    <mergeCell ref="O22:P23"/>
+    <mergeCell ref="Q22:R23"/>
+    <mergeCell ref="S22:T23"/>
+    <mergeCell ref="N20:O21"/>
+    <mergeCell ref="P20:Q21"/>
+    <mergeCell ref="R20:S21"/>
+    <mergeCell ref="T20:U21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:P18"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="H20:I21"/>
+    <mergeCell ref="J20:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>